<commit_message>
HW 2 and KH
</commit_message>
<xml_diff>
--- a/Professional/1-Internship-Applications/Internship-Applications.xlsx
+++ b/Professional/1-Internship-Applications/Internship-Applications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\Folder\Professional\1-Internship-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40920EA-3C8D-4B84-AD66-12AEF6720897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8EF2AE-1B8B-4292-B81D-2BB13D73BD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" activeTab="2" xr2:uid="{EE9BE8F8-8993-434B-83DF-83945B9CA987}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>Company</t>
   </si>
@@ -269,6 +269,21 @@
   </si>
   <si>
     <t>2026 Modeling and Simulation Graduate Intern - Communications and Ground Architectures</t>
+  </si>
+  <si>
+    <t>2025 Emerging Missions Flight Dynamics Graduate Intern</t>
+  </si>
+  <si>
+    <t>2025 Systems, Performance, Estimation and Algorithms Graduate Intern</t>
+  </si>
+  <si>
+    <t>2026 Space Mission Analysis and Operations Graduate Intern</t>
+  </si>
+  <si>
+    <t>Systems Engineering Intern (Summer 2026)</t>
+  </si>
+  <si>
+    <t>Muon</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1661,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2051,18 +2066,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDDC358-AE57-4406-AD58-BCD1B1BBA41C}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2087,10 +2105,10 @@
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -2100,10 +2118,10 @@
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -2116,7 +2134,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -2126,10 +2144,10 @@
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -2139,10 +2157,10 @@
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -2152,10 +2170,10 @@
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -2164,8 +2182,12 @@
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
+      <c r="A8" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -2173,8 +2195,12 @@
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -2182,8 +2208,12 @@
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -2191,8 +2221,12 @@
       <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -2406,25 +2440,20 @@
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
     </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{0CA6EBB7-A43F-47D0-B3BB-FC2075664D58}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{C532AD84-CBC3-4A09-87F8-2E8428189E58}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{4BA0AB06-0EC3-4E14-BD45-D969A1BC0E0E}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{48384DE1-9480-40A5-8069-09F95D419795}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{0B9814E7-0CAB-44B1-A793-234317FA4DB2}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{20291FE1-08EC-409B-B6EC-EB63108E8403}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{65516654-4B3C-471C-A625-3BF235314F9A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{224D4B3D-E82E-4B15-9423-539BFD8B9515}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A6DE6E64-E488-465B-A0C5-0C16E1BEC1DF}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{F404176A-E4D7-4A46-89A2-DA32651C939C}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{6EEBC9C6-60D3-4ADD-A3CB-A0615F81D0BC}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{A022AB0D-A7AA-46B2-A73B-39341EBEAD7C}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{7D828841-55DC-4589-B6AA-0F776968734E}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{C5765DAE-FE31-4875-A27D-A2262FAED5E3}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{A9D39848-2743-469C-A565-17525A9058C7}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{ADB07E57-E7C7-4154-88A5-06539CEB6F61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KH and project updates
</commit_message>
<xml_diff>
--- a/Professional/1-Internship-Applications/Internship-Applications.xlsx
+++ b/Professional/1-Internship-Applications/Internship-Applications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\Folder\Professional\1-Internship-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8EF2AE-1B8B-4292-B81D-2BB13D73BD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB10840-192D-45FA-94A8-B6CAD8CD9C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" activeTab="2" xr2:uid="{EE9BE8F8-8993-434B-83DF-83945B9CA987}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>Company</t>
   </si>
@@ -284,6 +284,48 @@
   </si>
   <si>
     <t>Muon</t>
+  </si>
+  <si>
+    <t>2026 Navigation &amp; Positioning Systems Graduate Intern</t>
+  </si>
+  <si>
+    <t>Space Operations Engineering Intern (Summer 2026)</t>
+  </si>
+  <si>
+    <t>Impulse</t>
+  </si>
+  <si>
+    <t>Automation &amp; Controls Engineering Intern (Summer 2026)</t>
+  </si>
+  <si>
+    <t>GNC Engineering Spring 2026 Intern</t>
+  </si>
+  <si>
+    <t>Reditus</t>
+  </si>
+  <si>
+    <t>Space GNC Graduate Intern – Summer 2026</t>
+  </si>
+  <si>
+    <t>Draper</t>
+  </si>
+  <si>
+    <t>Navigation &amp; Tracking Engineering Intern</t>
+  </si>
+  <si>
+    <t>Internship - Far ranges safety analysis and modelization</t>
+  </si>
+  <si>
+    <t>MaiaSpace</t>
+  </si>
+  <si>
+    <t>Barrios</t>
+  </si>
+  <si>
+    <t>Summer Computer Science / Engineering Intern - Summer 2026</t>
+  </si>
+  <si>
+    <t>Summer Engineering Intern - Summer 2026</t>
   </si>
 </sst>
 </file>
@@ -457,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -513,6 +555,7 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -851,7 +894,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1048576"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1658,16 +1701,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01067E36-577F-4CCF-A15A-7E93E9863B48}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.54296875" customWidth="1"/>
     <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.26953125" bestFit="1" customWidth="1"/>
@@ -1749,50 +1792,66 @@
       <c r="B5" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20">
+        <v>45923</v>
+      </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+        <v>86</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20">
+        <v>45923</v>
+      </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20">
+        <v>45924</v>
+      </c>
+      <c r="E7" s="19"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="A8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20">
+        <v>45925</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1800,8 +1859,12 @@
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -2051,14 +2114,44 @@
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
     </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DB3431C2-2A27-4BFA-98C1-BBC0A9DE9097}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{54B1B0BB-CA1A-4791-BA05-93341442D8B2}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{39FB14AD-4F2C-4C72-B805-A17EA6F01E27}"/>
     <hyperlink ref="B5" r:id="rId4" location="jobopenings" xr:uid="{5710F4E4-D945-4233-9AED-4A8872E0F547}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{060CDB43-B92B-42FC-A439-B13341915E3E}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{71856046-CC13-444F-85FE-3C6B29991BCA}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{060CDB43-B92B-42FC-A439-B13341915E3E}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{71856046-CC13-444F-85FE-3C6B29991BCA}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{57DB3993-1C06-41DD-B700-749E8DF154F5}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{E32BA8B3-0345-4D80-A929-8938D9E1A981}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{6F6C53CE-B5B0-4B1F-827B-BF333E73A649}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2066,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDDC358-AE57-4406-AD58-BCD1B1BBA41C}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2078,6 +2171,7 @@
     <col min="2" max="2" width="82" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2110,8 +2204,10 @@
       <c r="B2" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20">
+        <v>45923</v>
+      </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -2123,8 +2219,10 @@
       <c r="B3" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20">
+        <v>45923</v>
+      </c>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
@@ -2136,8 +2234,10 @@
       <c r="B4" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20">
+        <v>45923</v>
+      </c>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -2149,8 +2249,10 @@
       <c r="B5" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20">
+        <v>45923</v>
+      </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2162,89 +2264,111 @@
       <c r="B6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20">
+        <v>45923</v>
+      </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+        <v>82</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20">
+        <v>45923</v>
+      </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+        <v>66</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20">
+        <v>45923</v>
+      </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+        <v>80</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20">
+        <v>45923</v>
+      </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+        <v>69</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20">
+        <v>45924</v>
+      </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+        <v>88</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20">
+        <v>45924</v>
+      </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="A12" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20">
+        <v>45924</v>
+      </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -2252,8 +2376,12 @@
       <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -2261,8 +2389,12 @@
       <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>94</v>
+      </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -2270,8 +2402,12 @@
       <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>95</v>
+      </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -2279,8 +2415,12 @@
       <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -2288,8 +2428,12 @@
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -2440,6 +2584,33 @@
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
     </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{65516654-4B3C-471C-A625-3BF235314F9A}"/>
@@ -2447,13 +2618,20 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{A6DE6E64-E488-465B-A0C5-0C16E1BEC1DF}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{F404176A-E4D7-4A46-89A2-DA32651C939C}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{6EEBC9C6-60D3-4ADD-A3CB-A0615F81D0BC}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{A022AB0D-A7AA-46B2-A73B-39341EBEAD7C}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{7D828841-55DC-4589-B6AA-0F776968734E}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{C5765DAE-FE31-4875-A27D-A2262FAED5E3}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{A9D39848-2743-469C-A565-17525A9058C7}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{ADB07E57-E7C7-4154-88A5-06539CEB6F61}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{A022AB0D-A7AA-46B2-A73B-39341EBEAD7C}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{5F3E54D5-859C-45C5-A8D9-297779DDA797}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{143F0765-DF28-471B-8D3A-CE610EB17DFD}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{E4DAC39F-8A9E-4E8D-8472-1B1A0AD74C60}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{FD11A5B1-F66E-453C-9FC6-B90A724906CB}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{F393C037-1537-4C87-AD5B-36AE2B3203B8}"/>
+    <hyperlink ref="B11" r:id="rId12" xr:uid="{7A08AC69-6B92-4356-90DB-5EAE32F40529}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{EFA622C7-ACD9-4B6E-9975-F370FDAB3F7D}"/>
+    <hyperlink ref="B9" r:id="rId14" xr:uid="{D7100AAD-6E23-4005-89A2-72EB7558F570}"/>
+    <hyperlink ref="B10" r:id="rId15" xr:uid="{149ECCB6-01DA-465B-B56E-883D29936924}"/>
+    <hyperlink ref="B15" r:id="rId16" xr:uid="{542715D7-C1DB-43AB-9B51-7E6626E827DD}"/>
+    <hyperlink ref="B16" r:id="rId17" xr:uid="{201086E8-D8FA-493E-9E2F-78174CA96BE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First draft of essay
</commit_message>
<xml_diff>
--- a/Professional/1-Internship-Applications/Internship-Applications.xlsx
+++ b/Professional/1-Internship-Applications/Internship-Applications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\Folder\Professional\1-Internship-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB10840-192D-45FA-94A8-B6CAD8CD9C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E5AC7-D332-46A9-8937-EA3140DD6BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" activeTab="2" xr2:uid="{EE9BE8F8-8993-434B-83DF-83945B9CA987}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Fall-2025" sheetId="1" r:id="rId1"/>
     <sheet name="Spring-2026" sheetId="2" r:id="rId2"/>
     <sheet name="Summer-2026" sheetId="3" r:id="rId3"/>
+    <sheet name="Misc" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>Company</t>
   </si>
@@ -295,9 +296,6 @@
     <t>Impulse</t>
   </si>
   <si>
-    <t>Automation &amp; Controls Engineering Intern (Summer 2026)</t>
-  </si>
-  <si>
     <t>GNC Engineering Spring 2026 Intern</t>
   </si>
   <si>
@@ -326,6 +324,24 @@
   </si>
   <si>
     <t>Summer Engineering Intern - Summer 2026</t>
+  </si>
+  <si>
+    <t>Internshp</t>
+  </si>
+  <si>
+    <t>NASA JPL</t>
+  </si>
+  <si>
+    <t>2026 Remote Sensing Architecture Performance Graduate Intern</t>
+  </si>
+  <si>
+    <t>2026 Space Systems Architect Graduate Intern</t>
+  </si>
+  <si>
+    <t>Guidance Navigation &amp; Control (GNC) Intern – Summer 2026</t>
+  </si>
+  <si>
+    <t>K2</t>
   </si>
 </sst>
 </file>
@@ -894,7 +910,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1701,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01067E36-577F-4CCF-A15A-7E93E9863B48}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1802,10 +1818,10 @@
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="20">
@@ -1832,10 +1848,10 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="20">
@@ -1847,23 +1863,25 @@
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+        <v>95</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20">
+        <v>45926</v>
+      </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -1872,8 +1890,12 @@
       <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -2141,17 +2163,27 @@
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
     </row>
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DB3431C2-2A27-4BFA-98C1-BBC0A9DE9097}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{54B1B0BB-CA1A-4791-BA05-93341442D8B2}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{39FB14AD-4F2C-4C72-B805-A17EA6F01E27}"/>
     <hyperlink ref="B5" r:id="rId4" location="jobopenings" xr:uid="{5710F4E4-D945-4233-9AED-4A8872E0F547}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{060CDB43-B92B-42FC-A439-B13341915E3E}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{71856046-CC13-444F-85FE-3C6B29991BCA}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{060CDB43-B92B-42FC-A439-B13341915E3E}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{71856046-CC13-444F-85FE-3C6B29991BCA}"/>
     <hyperlink ref="B6" r:id="rId7" xr:uid="{57DB3993-1C06-41DD-B700-749E8DF154F5}"/>
     <hyperlink ref="B7" r:id="rId8" xr:uid="{E32BA8B3-0345-4D80-A929-8938D9E1A981}"/>
     <hyperlink ref="B8" r:id="rId9" xr:uid="{6F6C53CE-B5B0-4B1F-827B-BF333E73A649}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{0AD36ED9-F961-46E3-BA5C-39BF3741F68A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2159,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DDDC358-AE57-4406-AD58-BCD1B1BBA41C}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2334,10 +2366,10 @@
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="20">
@@ -2349,10 +2381,10 @@
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>89</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>90</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20">
@@ -2364,75 +2396,85 @@
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="17" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+        <v>95</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20">
+        <v>45926</v>
+      </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="17" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+        <v>97</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20">
+        <v>45929</v>
+      </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="17" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+        <v>98</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20">
+        <v>45929</v>
+      </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20">
+        <v>45930</v>
+      </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+        <v>99</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20">
+        <v>45930</v>
+      </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="17" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -2441,8 +2483,12 @@
       <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -2450,8 +2496,12 @@
       <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -2459,8 +2509,12 @@
       <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>75</v>
+      </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -2610,6 +2664,33 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2620,18 +2701,427 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{6EEBC9C6-60D3-4ADD-A3CB-A0615F81D0BC}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{A022AB0D-A7AA-46B2-A73B-39341EBEAD7C}"/>
     <hyperlink ref="B7" r:id="rId7" xr:uid="{5F3E54D5-859C-45C5-A8D9-297779DDA797}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{143F0765-DF28-471B-8D3A-CE610EB17DFD}"/>
-    <hyperlink ref="B14" r:id="rId9" xr:uid="{E4DAC39F-8A9E-4E8D-8472-1B1A0AD74C60}"/>
-    <hyperlink ref="B17" r:id="rId10" xr:uid="{FD11A5B1-F66E-453C-9FC6-B90A724906CB}"/>
-    <hyperlink ref="B18" r:id="rId11" xr:uid="{F393C037-1537-4C87-AD5B-36AE2B3203B8}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{7A08AC69-6B92-4356-90DB-5EAE32F40529}"/>
-    <hyperlink ref="B12" r:id="rId13" xr:uid="{EFA622C7-ACD9-4B6E-9975-F370FDAB3F7D}"/>
-    <hyperlink ref="B9" r:id="rId14" xr:uid="{D7100AAD-6E23-4005-89A2-72EB7558F570}"/>
-    <hyperlink ref="B10" r:id="rId15" xr:uid="{149ECCB6-01DA-465B-B56E-883D29936924}"/>
-    <hyperlink ref="B15" r:id="rId16" xr:uid="{542715D7-C1DB-43AB-9B51-7E6626E827DD}"/>
-    <hyperlink ref="B16" r:id="rId17" xr:uid="{201086E8-D8FA-493E-9E2F-78174CA96BE2}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{143F0765-DF28-471B-8D3A-CE610EB17DFD}"/>
+    <hyperlink ref="B20" r:id="rId9" xr:uid="{FD11A5B1-F66E-453C-9FC6-B90A724906CB}"/>
+    <hyperlink ref="B21" r:id="rId10" xr:uid="{F393C037-1537-4C87-AD5B-36AE2B3203B8}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{7A08AC69-6B92-4356-90DB-5EAE32F40529}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{EFA622C7-ACD9-4B6E-9975-F370FDAB3F7D}"/>
+    <hyperlink ref="B9" r:id="rId13" xr:uid="{D7100AAD-6E23-4005-89A2-72EB7558F570}"/>
+    <hyperlink ref="B10" r:id="rId14" xr:uid="{149ECCB6-01DA-465B-B56E-883D29936924}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{542715D7-C1DB-43AB-9B51-7E6626E827DD}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{201086E8-D8FA-493E-9E2F-78174CA96BE2}"/>
+    <hyperlink ref="B13" r:id="rId17" xr:uid="{4FFE44E0-0931-47A8-845E-ED8E1BD917C5}"/>
+    <hyperlink ref="B14" r:id="rId18" xr:uid="{97A4AE2D-75C0-4E08-B95F-BCDCC3BF1BDD}"/>
+    <hyperlink ref="B15" r:id="rId19" xr:uid="{D1169158-49D0-4677-BFB3-C92DE478275F}"/>
+    <hyperlink ref="B17" r:id="rId20" xr:uid="{EC1BB916-C153-49BF-A905-D43C566DAF0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72518C38-8093-481F-841A-834F90269DF5}">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update PD Soros Essay
</commit_message>
<xml_diff>
--- a/Professional/1-Internship-Applications/Internship-Applications.xlsx
+++ b/Professional/1-Internship-Applications/Internship-Applications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\Folder\Professional\1-Internship-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550408B-C890-4530-AD19-2D4D195AB668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763AD727-5B9F-4C48-830B-78C7E38E6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" activeTab="2" xr2:uid="{EE9BE8F8-8993-434B-83DF-83945B9CA987}"/>
   </bookViews>
@@ -2326,7 +2326,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2649,7 +2649,9 @@
       <c r="D15" s="20">
         <v>45929</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="22">
+        <v>0</v>
+      </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>

</xml_diff>